<commit_message>
added new functions. Added allure plugins.
</commit_message>
<xml_diff>
--- a/3PI/testdata/Testdata.xlsx
+++ b/3PI/testdata/Testdata.xlsx
@@ -83,10 +83,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,7 +366,7 @@
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -379,17 +379,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>TestCaseName</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>MethodName</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
@@ -647,9 +647,8 @@
           <t>Expected_date</t>
         </is>
       </c>
-      <c r="C16" s="5">
-        <f>TODAY()</f>
-        <v/>
+      <c r="C16" s="6" t="n">
+        <v>44196</v>
       </c>
     </row>
     <row r="17">
@@ -733,7 +732,7 @@
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>25299</t>
+          <t>25302</t>
         </is>
       </c>
     </row>

</xml_diff>